<commit_message>
work on minimum wage merges
</commit_message>
<xml_diff>
--- a/Supplemental Data/city_minwages.xlsx
+++ b/Supplemental Data/city_minwages.xlsx
@@ -8,18 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/velas/Documents/GU/Fall2024/Thesis/Work/Supplemental Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F66FB6F-5404-C942-879E-1980B75BE0CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39CF4D8-48D7-094F-ADEF-D632BA0BC37B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" xr2:uid="{6E60D62A-27A0-1E4F-AB05-101D0D1C9C2F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14320" windowHeight="16320" xr2:uid="{6F30BD62-F3FC-3043-BED6-D5928128AF6B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="city_minwages" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -83,9 +80,6 @@
     <t>Foster City city, California</t>
   </si>
   <si>
-    <t>Freemont city, California</t>
-  </si>
-  <si>
     <t>Half Moon Bay city, California</t>
   </si>
   <si>
@@ -195,13 +189,16 @@
   </si>
   <si>
     <t>West Hollywood city, California</t>
+  </si>
+  <si>
+    <t>Fremont city, California</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -210,22 +207,315 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -234,286 +524,203 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
+      <left/>
+      <right/>
       <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
+      <bottom style="thick">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
+      <left/>
+      <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
-        <color rgb="FF000000"/>
+        <color theme="4" tint="0.39997558519241921"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="hair">
-        <color indexed="64"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="hair">
-        <color rgb="FF000000"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top/>
-      <bottom style="hair">
-        <color indexed="64"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="hair">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -844,20 +1051,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C900D83-A941-354E-BE15-2763031ECB90}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB93855B-9727-BD47-A4D0-2FB6E7AC4D16}">
   <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O29" sqref="O29"/>
+      <selection pane="topRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="47.1640625" customWidth="1"/>
+    <col min="1" max="1" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -901,9 +1108,33 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>1</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>8</v>
+      </c>
+      <c r="F2">
+        <v>9</v>
+      </c>
+      <c r="G2">
+        <v>9</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+      <c r="I2">
+        <v>10</v>
       </c>
       <c r="J2">
         <v>11</v>
@@ -921,9 +1152,15 @@
         <v>16.52</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>2</v>
+      </c>
+      <c r="B3">
+        <v>7.5</v>
+      </c>
+      <c r="C3">
+        <v>7.5</v>
       </c>
       <c r="D3">
         <v>7.5</v>
@@ -947,21 +1184,42 @@
         <v>8.5</v>
       </c>
       <c r="K3">
-        <v>8.5</v>
+        <v>9</v>
       </c>
       <c r="L3">
-        <v>8.5</v>
+        <v>9</v>
       </c>
       <c r="M3">
-        <v>8.5</v>
+        <v>9</v>
       </c>
       <c r="N3">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>3</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>8</v>
+      </c>
+      <c r="F4">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>9</v>
+      </c>
+      <c r="H4">
+        <v>10</v>
       </c>
       <c r="I4">
         <v>10.5</v>
@@ -982,9 +1240,27 @@
         <v>16.75</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>4</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>8</v>
+      </c>
+      <c r="F5">
+        <v>9</v>
+      </c>
+      <c r="G5">
+        <v>9</v>
       </c>
       <c r="H5">
         <v>11</v>
@@ -1008,9 +1284,36 @@
         <v>16.989999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>5</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>8</v>
+      </c>
+      <c r="F6">
+        <v>9</v>
+      </c>
+      <c r="G6">
+        <v>9</v>
+      </c>
+      <c r="H6">
+        <v>10</v>
+      </c>
+      <c r="I6">
+        <v>10</v>
+      </c>
+      <c r="J6">
+        <v>11</v>
       </c>
       <c r="K6">
         <v>11</v>
@@ -1025,9 +1328,21 @@
         <v>16.47</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>6</v>
+      </c>
+      <c r="B7">
+        <v>8.25</v>
+      </c>
+      <c r="C7">
+        <v>8.25</v>
+      </c>
+      <c r="D7">
+        <v>8.25</v>
+      </c>
+      <c r="E7">
+        <v>8.25</v>
       </c>
       <c r="F7">
         <v>8.25</v>
@@ -1057,9 +1372,27 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>7</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="E8">
+        <v>8</v>
+      </c>
+      <c r="F8">
+        <v>9</v>
+      </c>
+      <c r="G8">
+        <v>9</v>
       </c>
       <c r="H8">
         <v>10</v>
@@ -1083,9 +1416,33 @@
         <v>17.2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>8</v>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>8</v>
+      </c>
+      <c r="F9">
+        <v>9</v>
+      </c>
+      <c r="G9">
+        <v>9</v>
+      </c>
+      <c r="H9">
+        <v>10</v>
+      </c>
+      <c r="I9">
+        <v>10</v>
       </c>
       <c r="J9">
         <v>11</v>
@@ -1103,9 +1460,36 @@
         <v>16.07</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="21" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>9</v>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>7.25</v>
+      </c>
+      <c r="C10">
+        <v>7.36</v>
+      </c>
+      <c r="D10">
+        <v>7.64</v>
+      </c>
+      <c r="E10">
+        <v>7.78</v>
+      </c>
+      <c r="F10">
+        <v>8</v>
+      </c>
+      <c r="G10">
+        <v>8.23</v>
+      </c>
+      <c r="H10">
+        <v>8.31</v>
+      </c>
+      <c r="I10">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="J10">
+        <v>10.199999999999999</v>
       </c>
       <c r="K10">
         <v>11.1</v>
@@ -1120,9 +1504,36 @@
         <v>15.87</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>10</v>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="D11">
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <v>8</v>
+      </c>
+      <c r="F11">
+        <v>9</v>
+      </c>
+      <c r="G11">
+        <v>9</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="I11">
+        <v>10</v>
+      </c>
+      <c r="J11">
+        <v>11</v>
       </c>
       <c r="K11">
         <v>12</v>
@@ -1138,8 +1549,23 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" t="s">
         <v>11</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>8</v>
+      </c>
+      <c r="D12">
+        <v>8</v>
+      </c>
+      <c r="E12">
+        <v>8</v>
+      </c>
+      <c r="F12">
+        <v>9</v>
       </c>
       <c r="G12">
         <v>10</v>
@@ -1166,9 +1592,21 @@
         <v>17.350000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>12</v>
+      </c>
+      <c r="B13">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>8</v>
+      </c>
+      <c r="D13">
+        <v>8</v>
+      </c>
+      <c r="E13">
+        <v>8</v>
       </c>
       <c r="F13">
         <v>9</v>
@@ -1198,9 +1636,27 @@
         <v>17.68</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>13</v>
+      </c>
+      <c r="B14">
+        <v>7.25</v>
+      </c>
+      <c r="C14">
+        <v>7.35</v>
+      </c>
+      <c r="D14">
+        <v>7.65</v>
+      </c>
+      <c r="E14">
+        <v>7.8</v>
+      </c>
+      <c r="F14">
+        <v>7.9</v>
+      </c>
+      <c r="G14">
+        <v>8.0500000000000007</v>
       </c>
       <c r="H14">
         <v>10</v>
@@ -1225,8 +1681,38 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="10" t="s">
+      <c r="A15" t="s">
         <v>14</v>
+      </c>
+      <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>8</v>
+      </c>
+      <c r="D15">
+        <v>8</v>
+      </c>
+      <c r="E15">
+        <v>8</v>
+      </c>
+      <c r="F15">
+        <v>9</v>
+      </c>
+      <c r="G15">
+        <v>9</v>
+      </c>
+      <c r="H15">
+        <v>10</v>
+      </c>
+      <c r="I15">
+        <v>10</v>
+      </c>
+      <c r="J15">
+        <v>11</v>
+      </c>
+      <c r="K15">
+        <v>12</v>
       </c>
       <c r="L15">
         <v>14</v>
@@ -1238,9 +1724,36 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>15</v>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>8</v>
+      </c>
+      <c r="D16">
+        <v>8</v>
+      </c>
+      <c r="E16">
+        <v>8</v>
+      </c>
+      <c r="F16">
+        <v>9</v>
+      </c>
+      <c r="G16">
+        <v>9</v>
+      </c>
+      <c r="H16">
+        <v>10</v>
+      </c>
+      <c r="I16">
+        <v>10</v>
+      </c>
+      <c r="J16">
+        <v>11</v>
       </c>
       <c r="K16">
         <v>11</v>
@@ -1255,9 +1768,36 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
-        <v>16</v>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>8</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+      <c r="E17">
+        <v>8</v>
+      </c>
+      <c r="F17">
+        <v>9</v>
+      </c>
+      <c r="G17">
+        <v>9</v>
+      </c>
+      <c r="H17">
+        <v>10</v>
+      </c>
+      <c r="I17">
+        <v>10</v>
+      </c>
+      <c r="J17">
+        <v>11</v>
       </c>
       <c r="K17">
         <v>12</v>
@@ -1272,9 +1812,36 @@
         <v>16.45</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
-        <v>17</v>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <v>8</v>
+      </c>
+      <c r="D18">
+        <v>8</v>
+      </c>
+      <c r="E18">
+        <v>8</v>
+      </c>
+      <c r="F18">
+        <v>9</v>
+      </c>
+      <c r="G18">
+        <v>9</v>
+      </c>
+      <c r="H18">
+        <v>10</v>
+      </c>
+      <c r="I18">
+        <v>10</v>
+      </c>
+      <c r="J18">
+        <v>11</v>
       </c>
       <c r="K18">
         <v>12</v>
@@ -1289,9 +1856,21 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
-        <v>18</v>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>7.5</v>
+      </c>
+      <c r="C19">
+        <v>7.5</v>
+      </c>
+      <c r="D19">
+        <v>7.5</v>
+      </c>
+      <c r="E19">
+        <v>7.5</v>
       </c>
       <c r="F19">
         <v>7.5</v>
@@ -1321,9 +1900,27 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
-        <v>19</v>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>8</v>
+      </c>
+      <c r="D20">
+        <v>8</v>
+      </c>
+      <c r="E20">
+        <v>8</v>
+      </c>
+      <c r="F20">
+        <v>9</v>
+      </c>
+      <c r="G20">
+        <v>9</v>
       </c>
       <c r="H20">
         <v>10</v>
@@ -1347,9 +1944,27 @@
         <v>17.2</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>20</v>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>8</v>
+      </c>
+      <c r="C21">
+        <v>8</v>
+      </c>
+      <c r="D21">
+        <v>8</v>
+      </c>
+      <c r="E21">
+        <v>8</v>
+      </c>
+      <c r="F21">
+        <v>9</v>
+      </c>
+      <c r="G21">
+        <v>9</v>
       </c>
       <c r="H21">
         <v>10</v>
@@ -1373,9 +1988,27 @@
         <v>16.04</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>21</v>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>8</v>
+      </c>
+      <c r="C22">
+        <v>8</v>
+      </c>
+      <c r="D22">
+        <v>8</v>
+      </c>
+      <c r="E22">
+        <v>8</v>
+      </c>
+      <c r="F22">
+        <v>9</v>
+      </c>
+      <c r="G22">
+        <v>9</v>
       </c>
       <c r="H22">
         <v>10</v>
@@ -1399,9 +2032,36 @@
         <v>15.96</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
-        <v>22</v>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <v>8</v>
+      </c>
+      <c r="D23">
+        <v>8</v>
+      </c>
+      <c r="E23">
+        <v>8</v>
+      </c>
+      <c r="F23">
+        <v>9</v>
+      </c>
+      <c r="G23">
+        <v>9</v>
+      </c>
+      <c r="H23">
+        <v>10</v>
+      </c>
+      <c r="I23">
+        <v>10</v>
+      </c>
+      <c r="J23">
+        <v>11</v>
       </c>
       <c r="K23">
         <v>11</v>
@@ -1413,12 +2073,30 @@
         <v>15.75</v>
       </c>
       <c r="N23">
-        <v>15</v>
+        <v>16.5</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>23</v>
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>8</v>
+      </c>
+      <c r="C24">
+        <v>8</v>
+      </c>
+      <c r="D24">
+        <v>8</v>
+      </c>
+      <c r="E24">
+        <v>8</v>
+      </c>
+      <c r="F24">
+        <v>9</v>
+      </c>
+      <c r="G24">
+        <v>9</v>
       </c>
       <c r="H24">
         <v>10</v>
@@ -1442,9 +2120,30 @@
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
-        <v>24</v>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>7.25</v>
+      </c>
+      <c r="C25">
+        <v>7.25</v>
+      </c>
+      <c r="D25">
+        <v>7.25</v>
+      </c>
+      <c r="E25">
+        <v>7.25</v>
+      </c>
+      <c r="F25">
+        <v>7.25</v>
+      </c>
+      <c r="G25">
+        <v>7.25</v>
+      </c>
+      <c r="H25">
+        <v>7.25</v>
       </c>
       <c r="I25">
         <v>7.75</v>
@@ -1465,9 +2164,24 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
-        <v>25</v>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>8</v>
+      </c>
+      <c r="C26">
+        <v>8</v>
+      </c>
+      <c r="D26">
+        <v>8</v>
+      </c>
+      <c r="E26">
+        <v>8</v>
+      </c>
+      <c r="F26">
+        <v>9</v>
       </c>
       <c r="G26">
         <v>10.3</v>
@@ -1494,12 +2208,39 @@
         <v>18.149999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
-        <v>26</v>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>8</v>
+      </c>
+      <c r="D27">
+        <v>8</v>
+      </c>
+      <c r="E27">
+        <v>8</v>
+      </c>
+      <c r="F27">
+        <v>9</v>
+      </c>
+      <c r="G27">
+        <v>9</v>
+      </c>
+      <c r="H27">
+        <v>10</v>
+      </c>
+      <c r="I27">
+        <v>10</v>
+      </c>
+      <c r="J27">
+        <v>11</v>
       </c>
       <c r="K27">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L27">
         <v>14</v>
@@ -1511,9 +2252,21 @@
         <v>15.53</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>27</v>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>8</v>
+      </c>
+      <c r="C28">
+        <v>8</v>
+      </c>
+      <c r="D28">
+        <v>8</v>
+      </c>
+      <c r="E28">
+        <v>8</v>
       </c>
       <c r="F28">
         <v>9</v>
@@ -1543,9 +2296,24 @@
         <v>15.97</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>28</v>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>8</v>
+      </c>
+      <c r="C29">
+        <v>8</v>
+      </c>
+      <c r="D29">
+        <v>8</v>
+      </c>
+      <c r="E29">
+        <v>8</v>
+      </c>
+      <c r="F29">
+        <v>9</v>
       </c>
       <c r="G29">
         <v>9</v>
@@ -1572,9 +2340,27 @@
         <v>17.25</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="16" t="s">
-        <v>29</v>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>8</v>
+      </c>
+      <c r="C30">
+        <v>8</v>
+      </c>
+      <c r="D30">
+        <v>8</v>
+      </c>
+      <c r="E30">
+        <v>8</v>
+      </c>
+      <c r="F30">
+        <v>9</v>
+      </c>
+      <c r="G30">
+        <v>9</v>
       </c>
       <c r="H30">
         <v>10</v>
@@ -1598,9 +2384,36 @@
         <v>16.11</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="15" t="s">
-        <v>30</v>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>8</v>
+      </c>
+      <c r="C31">
+        <v>8</v>
+      </c>
+      <c r="D31">
+        <v>8</v>
+      </c>
+      <c r="E31">
+        <v>8</v>
+      </c>
+      <c r="F31">
+        <v>9</v>
+      </c>
+      <c r="G31">
+        <v>9</v>
+      </c>
+      <c r="H31">
+        <v>10</v>
+      </c>
+      <c r="I31">
+        <v>10</v>
+      </c>
+      <c r="J31">
+        <v>11</v>
       </c>
       <c r="K31">
         <v>11</v>
@@ -1615,9 +2428,24 @@
         <v>17.059999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
-        <v>31</v>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>7.5</v>
+      </c>
+      <c r="C32">
+        <v>7.5</v>
+      </c>
+      <c r="D32">
+        <v>7.5</v>
+      </c>
+      <c r="E32">
+        <v>7.5</v>
+      </c>
+      <c r="F32">
+        <v>7.5</v>
       </c>
       <c r="G32">
         <v>7.5</v>
@@ -1644,9 +2472,33 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
-        <v>32</v>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>8</v>
+      </c>
+      <c r="C33">
+        <v>8</v>
+      </c>
+      <c r="D33">
+        <v>8</v>
+      </c>
+      <c r="E33">
+        <v>8</v>
+      </c>
+      <c r="F33">
+        <v>9</v>
+      </c>
+      <c r="G33">
+        <v>9</v>
+      </c>
+      <c r="H33">
+        <v>10</v>
+      </c>
+      <c r="I33">
+        <v>10</v>
       </c>
       <c r="J33">
         <v>10.5</v>
@@ -1664,9 +2516,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="13" t="s">
-        <v>33</v>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>8</v>
+      </c>
+      <c r="C34">
+        <v>8</v>
+      </c>
+      <c r="D34">
+        <v>8</v>
+      </c>
+      <c r="E34">
+        <v>8</v>
       </c>
       <c r="F34">
         <v>9</v>
@@ -1696,9 +2560,39 @@
         <v>16.170000000000002</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>34</v>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>7.5</v>
+      </c>
+      <c r="C35">
+        <v>7.5</v>
+      </c>
+      <c r="D35">
+        <v>7.5</v>
+      </c>
+      <c r="E35">
+        <v>7.5</v>
+      </c>
+      <c r="F35">
+        <v>7.5</v>
+      </c>
+      <c r="G35">
+        <v>7.5</v>
+      </c>
+      <c r="H35">
+        <v>7.5</v>
+      </c>
+      <c r="I35">
+        <v>9</v>
+      </c>
+      <c r="J35">
+        <v>10</v>
+      </c>
+      <c r="K35">
+        <v>12</v>
       </c>
       <c r="L35">
         <v>12.15</v>
@@ -1710,12 +2604,39 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="17" t="s">
-        <v>35</v>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>7.25</v>
+      </c>
+      <c r="C36">
+        <v>7.25</v>
+      </c>
+      <c r="D36">
+        <v>7.25</v>
+      </c>
+      <c r="E36">
+        <v>7.25</v>
+      </c>
+      <c r="F36">
+        <v>7.25</v>
+      </c>
+      <c r="G36">
+        <v>7.25</v>
+      </c>
+      <c r="H36">
+        <v>7.25</v>
+      </c>
+      <c r="I36">
+        <v>7.75</v>
+      </c>
+      <c r="J36">
+        <v>8.0399999999999991</v>
       </c>
       <c r="K36">
-        <v>8.0399999999999991</v>
+        <v>8.15</v>
       </c>
       <c r="L36">
         <v>11</v>
@@ -1727,9 +2648,36 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="14" t="s">
-        <v>36</v>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>8</v>
+      </c>
+      <c r="C37">
+        <v>8</v>
+      </c>
+      <c r="D37">
+        <v>8</v>
+      </c>
+      <c r="E37">
+        <v>8</v>
+      </c>
+      <c r="F37">
+        <v>9</v>
+      </c>
+      <c r="G37">
+        <v>9</v>
+      </c>
+      <c r="H37">
+        <v>10</v>
+      </c>
+      <c r="I37">
+        <v>10</v>
+      </c>
+      <c r="J37">
+        <v>11</v>
       </c>
       <c r="K37">
         <v>12</v>
@@ -1744,9 +2692,21 @@
         <v>16.32</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="13" t="s">
-        <v>37</v>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>8</v>
+      </c>
+      <c r="C38">
+        <v>8</v>
+      </c>
+      <c r="D38">
+        <v>8</v>
+      </c>
+      <c r="E38">
+        <v>8</v>
       </c>
       <c r="F38">
         <v>9</v>
@@ -1776,9 +2736,21 @@
         <v>16.3</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>38</v>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>8</v>
+      </c>
+      <c r="C39">
+        <v>8</v>
+      </c>
+      <c r="D39">
+        <v>8</v>
+      </c>
+      <c r="E39">
+        <v>8</v>
       </c>
       <c r="F39">
         <v>11.05</v>
@@ -1808,9 +2780,27 @@
         <v>16.989999999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="13" t="s">
-        <v>39</v>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>8</v>
+      </c>
+      <c r="C40">
+        <v>8</v>
+      </c>
+      <c r="D40">
+        <v>8</v>
+      </c>
+      <c r="E40">
+        <v>8</v>
+      </c>
+      <c r="F40">
+        <v>9</v>
+      </c>
+      <c r="G40">
+        <v>9</v>
       </c>
       <c r="H40">
         <v>10</v>
@@ -1834,9 +2824,27 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="13" t="s">
-        <v>40</v>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>8</v>
+      </c>
+      <c r="C41">
+        <v>8</v>
+      </c>
+      <c r="D41">
+        <v>8</v>
+      </c>
+      <c r="E41">
+        <v>8</v>
+      </c>
+      <c r="F41">
+        <v>9</v>
+      </c>
+      <c r="G41">
+        <v>9</v>
       </c>
       <c r="H41">
         <v>10</v>
@@ -1860,9 +2868,27 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="18" t="s">
-        <v>41</v>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>8</v>
+      </c>
+      <c r="C42">
+        <v>8</v>
+      </c>
+      <c r="D42">
+        <v>8</v>
+      </c>
+      <c r="E42">
+        <v>8</v>
+      </c>
+      <c r="F42">
+        <v>9</v>
+      </c>
+      <c r="G42">
+        <v>9</v>
       </c>
       <c r="H42">
         <v>10</v>
@@ -1886,9 +2912,24 @@
         <v>16.75</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="19" t="s">
-        <v>42</v>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43">
+        <v>8</v>
+      </c>
+      <c r="C43">
+        <v>8</v>
+      </c>
+      <c r="D43">
+        <v>8</v>
+      </c>
+      <c r="E43">
+        <v>8</v>
+      </c>
+      <c r="F43">
+        <v>9</v>
       </c>
       <c r="G43">
         <v>9</v>
@@ -1916,8 +2957,8 @@
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A44" s="20" t="s">
-        <v>43</v>
+      <c r="A44" t="s">
+        <v>42</v>
       </c>
       <c r="B44">
         <v>9.5</v>
@@ -1960,8 +3001,26 @@
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A45" s="15" t="s">
-        <v>44</v>
+      <c r="A45" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>8</v>
+      </c>
+      <c r="C45">
+        <v>8</v>
+      </c>
+      <c r="D45">
+        <v>8</v>
+      </c>
+      <c r="E45">
+        <v>8</v>
+      </c>
+      <c r="F45">
+        <v>9</v>
+      </c>
+      <c r="G45">
+        <v>9</v>
       </c>
       <c r="H45">
         <v>10</v>
@@ -1986,8 +3045,35 @@
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A46" s="15" t="s">
-        <v>45</v>
+      <c r="A46" t="s">
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <v>8</v>
+      </c>
+      <c r="C46">
+        <v>8</v>
+      </c>
+      <c r="D46">
+        <v>8</v>
+      </c>
+      <c r="E46">
+        <v>8</v>
+      </c>
+      <c r="F46">
+        <v>9</v>
+      </c>
+      <c r="G46">
+        <v>9</v>
+      </c>
+      <c r="H46">
+        <v>10</v>
+      </c>
+      <c r="I46">
+        <v>10</v>
+      </c>
+      <c r="J46">
+        <v>11</v>
       </c>
       <c r="K46">
         <v>12</v>
@@ -2002,9 +3088,21 @@
         <v>17.059999999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="9" t="s">
-        <v>46</v>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <v>8.5500000000000007</v>
+      </c>
+      <c r="C47">
+        <v>8.67</v>
+      </c>
+      <c r="D47">
+        <v>9.0399999999999991</v>
+      </c>
+      <c r="E47">
+        <v>9.19</v>
       </c>
       <c r="F47">
         <v>9.5399999999999991</v>
@@ -2034,9 +3132,36 @@
         <v>15.75</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="9" t="s">
-        <v>47</v>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <v>8</v>
+      </c>
+      <c r="C48">
+        <v>8</v>
+      </c>
+      <c r="D48">
+        <v>8</v>
+      </c>
+      <c r="E48">
+        <v>8</v>
+      </c>
+      <c r="F48">
+        <v>9</v>
+      </c>
+      <c r="G48">
+        <v>9</v>
+      </c>
+      <c r="H48">
+        <v>10</v>
+      </c>
+      <c r="I48">
+        <v>10</v>
+      </c>
+      <c r="J48">
+        <v>11</v>
       </c>
       <c r="K48">
         <v>11</v>
@@ -2051,12 +3176,39 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="9" t="s">
-        <v>48</v>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>47</v>
+      </c>
+      <c r="B49">
+        <v>8</v>
+      </c>
+      <c r="C49">
+        <v>8</v>
+      </c>
+      <c r="D49">
+        <v>8</v>
+      </c>
+      <c r="E49">
+        <v>8</v>
+      </c>
+      <c r="F49">
+        <v>9</v>
+      </c>
+      <c r="G49">
+        <v>9</v>
+      </c>
+      <c r="H49">
+        <v>10</v>
+      </c>
+      <c r="I49">
+        <v>10</v>
+      </c>
+      <c r="J49">
+        <v>11</v>
       </c>
       <c r="K49">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L49">
         <v>15.25</v>
@@ -2068,9 +3220,21 @@
         <v>16.7</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="13" t="s">
-        <v>49</v>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>48</v>
+      </c>
+      <c r="B50">
+        <v>8</v>
+      </c>
+      <c r="C50">
+        <v>8</v>
+      </c>
+      <c r="D50">
+        <v>8</v>
+      </c>
+      <c r="E50">
+        <v>8</v>
       </c>
       <c r="F50">
         <v>9</v>
@@ -2100,9 +3264,39 @@
         <v>17.95</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="9" t="s">
-        <v>50</v>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <v>7.25</v>
+      </c>
+      <c r="C51">
+        <v>7.35</v>
+      </c>
+      <c r="D51">
+        <v>7.65</v>
+      </c>
+      <c r="E51">
+        <v>7.8</v>
+      </c>
+      <c r="F51">
+        <v>7.9</v>
+      </c>
+      <c r="G51">
+        <v>8.0500000000000007</v>
+      </c>
+      <c r="H51">
+        <v>8.0500000000000007</v>
+      </c>
+      <c r="I51">
+        <v>10</v>
+      </c>
+      <c r="J51">
+        <v>10.5</v>
+      </c>
+      <c r="K51">
+        <v>12</v>
       </c>
       <c r="L51">
         <v>12.8</v>
@@ -2114,9 +3308,42 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="21" t="s">
-        <v>51</v>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>8.5500000000000007</v>
+      </c>
+      <c r="C52">
+        <v>8.67</v>
+      </c>
+      <c r="D52">
+        <v>9.0399999999999991</v>
+      </c>
+      <c r="E52">
+        <v>9.19</v>
+      </c>
+      <c r="F52">
+        <v>9.32</v>
+      </c>
+      <c r="G52">
+        <v>9.4700000000000006</v>
+      </c>
+      <c r="H52">
+        <v>9.4700000000000006</v>
+      </c>
+      <c r="I52">
+        <v>11</v>
+      </c>
+      <c r="J52">
+        <v>11.5</v>
+      </c>
+      <c r="K52">
+        <v>13.5</v>
+      </c>
+      <c r="L52">
+        <v>13.69</v>
       </c>
       <c r="M52">
         <v>15.74</v>
@@ -2126,8 +3353,41 @@
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A53" s="15" t="s">
-        <v>52</v>
+      <c r="A53" t="s">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>8</v>
+      </c>
+      <c r="C53">
+        <v>8</v>
+      </c>
+      <c r="D53">
+        <v>8</v>
+      </c>
+      <c r="E53">
+        <v>8</v>
+      </c>
+      <c r="F53">
+        <v>9</v>
+      </c>
+      <c r="G53">
+        <v>9</v>
+      </c>
+      <c r="H53">
+        <v>10</v>
+      </c>
+      <c r="I53">
+        <v>10</v>
+      </c>
+      <c r="J53">
+        <v>11</v>
+      </c>
+      <c r="K53">
+        <v>12</v>
+      </c>
+      <c r="L53">
+        <v>13</v>
       </c>
       <c r="M53">
         <v>16</v>
@@ -2137,6 +3397,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>